<commit_message>
running simulation on actual data implemented
it works
</commit_message>
<xml_diff>
--- a/assignments/three/gasstationdata33.xlsx
+++ b/assignments/three/gasstationdata33.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/m_a_yousif_student_tue_nl/Documents/Documents/Libros/Year 3/Q3/2WB50/StochasticSimulations/assignments/three/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_37116528DF68D0DEE54878D6425DCE3A87452277" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAA1EFCB-114E-4AA2-A88D-AE65ACD8C7C4}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_37116528DF68D0DEE54878D6425DCE3A87452277" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{317A73C8-1BCE-4577-9BF7-75DAA61A9C42}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,20 +419,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A411" workbookViewId="0">
+      <selection activeCell="G435" sqref="G435"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1"/>
-    <col min="7" max="7" width="31.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -475,7 +475,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -498,7 +498,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -521,7 +521,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -544,7 +544,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>7</v>
       </c>
@@ -567,7 +567,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -590,7 +590,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -613,7 +613,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -636,7 +636,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -659,7 +659,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -682,7 +682,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -705,7 +705,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -728,7 +728,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -751,7 +751,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -774,7 +774,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -797,7 +797,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -820,7 +820,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -843,7 +843,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -866,7 +866,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -889,7 +889,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -912,7 +912,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -935,7 +935,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -958,7 +958,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -981,7 +981,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>33</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>38</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>47</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>50</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>54</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>52</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>53</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>62</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>67</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>64</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>66</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>68</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>70</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>74</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>78</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>79</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>76</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>77</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>83</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>81</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>82</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>86</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>84</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>90</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>88</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>89</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>94</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>91</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>93</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>97</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>98</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>95</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>96</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>101</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>99</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>100</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>105</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>109</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>107</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>108</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>114</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>111</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>113</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>115</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>117</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>120</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>128</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>126</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>127</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>132</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>130</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>136</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>139</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>143</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>141</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>142</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>145</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>148</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>150</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>154</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>152</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>153</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>157</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>163</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>170</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>167</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>168</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>169</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>172</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>174</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>179</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>186</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>184</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>185</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>191</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>189</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>190</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>195</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>193</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>194</v>
       </c>
@@ -4983,7 +4983,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>199</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>197</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>202</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>206</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>204</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>208</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -5351,7 +5351,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>214</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>216</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>223</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>219</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>225</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>222</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>224</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>234</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>231</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>233</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>238</v>
       </c>
@@ -5926,7 +5926,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>237</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>240</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>239</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>245</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>243</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>248</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>249</v>
       </c>
@@ -6179,7 +6179,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>247</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -6225,7 +6225,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>252</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>251</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>254</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>253</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>258</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>255</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>257</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>264</v>
       </c>
@@ -6501,7 +6501,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -6524,7 +6524,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>262</v>
       </c>
@@ -6547,7 +6547,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>267</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>265</v>
       </c>
@@ -6616,7 +6616,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>273</v>
       </c>
@@ -6731,7 +6731,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>274</v>
       </c>
@@ -6754,7 +6754,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>272</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>277</v>
       </c>
@@ -6800,7 +6800,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>275</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -6869,7 +6869,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -7007,7 +7007,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>287</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -7053,7 +7053,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>285</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>289</v>
       </c>
@@ -7099,7 +7099,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>288</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>291</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>290</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -7237,7 +7237,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -7260,7 +7260,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>297</v>
       </c>
@@ -7283,7 +7283,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>296</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -7329,7 +7329,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -7352,7 +7352,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>301</v>
       </c>
@@ -7375,7 +7375,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>300</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>305</v>
       </c>
@@ -7444,7 +7444,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>303</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>304</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>307</v>
       </c>
@@ -7513,7 +7513,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>308</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>306</v>
       </c>
@@ -7559,7 +7559,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>310</v>
       </c>
@@ -7582,7 +7582,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>309</v>
       </c>
@@ -7605,7 +7605,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -7628,7 +7628,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>315</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>314</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>312</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>318</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>319</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>316</v>
       </c>
@@ -7789,7 +7789,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="321" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>317</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="322" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>320</v>
       </c>
@@ -7835,7 +7835,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>321</v>
       </c>
@@ -7858,7 +7858,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>323</v>
       </c>
@@ -7881,7 +7881,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>322</v>
       </c>
@@ -7904,7 +7904,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>326</v>
       </c>
@@ -7927,7 +7927,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="327" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>324</v>
       </c>
@@ -7950,7 +7950,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="328" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>325</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="329" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>327</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="330" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>329</v>
       </c>
@@ -8019,7 +8019,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="331" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>328</v>
       </c>
@@ -8042,7 +8042,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="332" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -8065,7 +8065,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="333" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>332</v>
       </c>
@@ -8088,7 +8088,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="334" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>331</v>
       </c>
@@ -8111,7 +8111,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="335" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>333</v>
       </c>
@@ -8134,7 +8134,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="336" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>336</v>
       </c>
@@ -8157,7 +8157,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>334</v>
       </c>
@@ -8180,7 +8180,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>337</v>
       </c>
@@ -8203,7 +8203,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>335</v>
       </c>
@@ -8226,7 +8226,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>338</v>
       </c>
@@ -8249,7 +8249,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>339</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>341</v>
       </c>
@@ -8318,7 +8318,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>343</v>
       </c>
@@ -8341,7 +8341,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>342</v>
       </c>
@@ -8364,7 +8364,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>344</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>346</v>
       </c>
@@ -8410,7 +8410,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>345</v>
       </c>
@@ -8433,7 +8433,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>347</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>349</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>348</v>
       </c>
@@ -8502,7 +8502,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>351</v>
       </c>
@@ -8525,7 +8525,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="353" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>350</v>
       </c>
@@ -8548,7 +8548,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="354" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -8571,7 +8571,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="355" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>354</v>
       </c>
@@ -8594,7 +8594,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="356" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>356</v>
       </c>
@@ -8617,7 +8617,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>353</v>
       </c>
@@ -8640,7 +8640,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="358" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>355</v>
       </c>
@@ -8663,7 +8663,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="359" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>358</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="360" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>357</v>
       </c>
@@ -8709,7 +8709,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>359</v>
       </c>
@@ -8732,7 +8732,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="362" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>360</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>361</v>
       </c>
@@ -8778,7 +8778,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>362</v>
       </c>
@@ -8801,7 +8801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>365</v>
       </c>
@@ -8824,7 +8824,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="366" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>364</v>
       </c>
@@ -8847,7 +8847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="367" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>363</v>
       </c>
@@ -8870,7 +8870,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="368" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>366</v>
       </c>
@@ -8893,7 +8893,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>370</v>
       </c>
@@ -8916,7 +8916,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>367</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>368</v>
       </c>
@@ -8962,7 +8962,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="372" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>369</v>
       </c>
@@ -8985,7 +8985,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="373" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>371</v>
       </c>
@@ -9008,7 +9008,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="374" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>372</v>
       </c>
@@ -9031,7 +9031,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="375" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>373</v>
       </c>
@@ -9054,7 +9054,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="376" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <v>374</v>
       </c>
@@ -9077,7 +9077,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="377" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <v>376</v>
       </c>
@@ -9100,7 +9100,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="378" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <v>375</v>
       </c>
@@ -9123,7 +9123,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="379" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <v>378</v>
       </c>
@@ -9146,7 +9146,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="380" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <v>377</v>
       </c>
@@ -9169,7 +9169,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="381" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <v>379</v>
       </c>
@@ -9192,7 +9192,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="382" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>381</v>
       </c>
@@ -9215,7 +9215,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="383" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
         <v>382</v>
       </c>
@@ -9238,7 +9238,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="384" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A384" s="1">
         <v>380</v>
       </c>
@@ -9261,7 +9261,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="385" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <v>383</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="386" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <v>385</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="387" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>386</v>
       </c>
@@ -9330,7 +9330,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="388" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>384</v>
       </c>
@@ -9353,7 +9353,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="389" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>387</v>
       </c>
@@ -9376,7 +9376,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="390" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>388</v>
       </c>
@@ -9399,7 +9399,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="391" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>389</v>
       </c>
@@ -9422,7 +9422,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="392" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>390</v>
       </c>
@@ -9445,7 +9445,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="393" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>391</v>
       </c>
@@ -9468,7 +9468,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="394" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>394</v>
       </c>
@@ -9491,7 +9491,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="395" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>392</v>
       </c>
@@ -9514,7 +9514,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="396" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>393</v>
       </c>
@@ -9537,7 +9537,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="397" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>395</v>
       </c>
@@ -9560,7 +9560,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="398" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>396</v>
       </c>
@@ -9583,7 +9583,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="399" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>397</v>
       </c>
@@ -9606,7 +9606,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="400" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>398</v>
       </c>
@@ -9629,7 +9629,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="401" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>399</v>
       </c>
@@ -9652,7 +9652,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="402" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>400</v>
       </c>
@@ -9675,7 +9675,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="403" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>401</v>
       </c>
@@ -9698,7 +9698,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="404" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>405</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="405" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>403</v>
       </c>
@@ -9744,7 +9744,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="406" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>402</v>
       </c>
@@ -9767,7 +9767,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="407" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>404</v>
       </c>
@@ -9790,7 +9790,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="408" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>406</v>
       </c>
@@ -9813,7 +9813,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="409" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>408</v>
       </c>
@@ -9836,7 +9836,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="410" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>409</v>
       </c>
@@ -9859,7 +9859,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="411" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>407</v>
       </c>
@@ -9882,7 +9882,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="412" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>411</v>
       </c>
@@ -9905,7 +9905,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="413" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
         <v>410</v>
       </c>
@@ -9928,7 +9928,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="414" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
         <v>412</v>
       </c>
@@ -9951,7 +9951,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="415" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <v>414</v>
       </c>
@@ -9974,7 +9974,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="416" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>415</v>
       </c>
@@ -9997,7 +9997,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="417" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>413</v>
       </c>
@@ -10020,7 +10020,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="418" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>418</v>
       </c>
@@ -10043,7 +10043,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="419" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <v>416</v>
       </c>
@@ -10066,7 +10066,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="420" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <v>419</v>
       </c>
@@ -10089,7 +10089,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="421" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>417</v>
       </c>
@@ -10112,7 +10112,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="422" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>420</v>
       </c>
@@ -10120,7 +10120,7 @@
         <v>420</v>
       </c>
       <c r="C422" s="2">
-        <v>45323.915982365987</v>
+        <v>45323.915983796294</v>
       </c>
       <c r="D422" t="s">
         <v>6</v>

</xml_diff>